<commit_message>
Added a comment and link
</commit_message>
<xml_diff>
--- a/ProjectStructure/planningText/Överblick punkter.xlsx
+++ b/ProjectStructure/planningText/Överblick punkter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffdb61f3ca5e596b/Gemensamma dokument/3.8. Skolan/WEBB-E-HANDEL/Repos/Webshop/diagrams/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisa Karnerfors\Desktop\Mediainstitutet\Systemutveckling och databasutveckling\Projektarbete - Systemutveckling och Databasteknik\Webshop\ProjectStructure\planningText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{F6681498-EF8F-468A-B336-4973DBEDF5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34B63BED-4DB1-45D4-B889-6BF5847D09E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD917F6-EC76-4A1E-B1FE-8DE377D35579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D4CAC9D2-5662-4D72-97CE-32DCF278DC94}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D4CAC9D2-5662-4D72-97CE-32DCF278DC94}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1467,9 +1467,6 @@
     <t>OK</t>
   </si>
   <si>
-    <t>Victor går igenom detta</t>
-  </si>
-  <si>
     <t>Uppdatera orderstatus: UPDATE `order`
 SET StatusID = 'CREC', CustRecDate = CURRENT_TIMESTAMP
 WHERE OrderID = 5</t>
@@ -1526,6 +1523,57 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Name, Description, UnitPrice, UnitsInStock, Image  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Victor gick igenom detta 3/2.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Länk till inspelningen:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://medieinstitutet-my.sharepoint.com/:v:/g/personal/lisa_karnerfors_medieinstitutet_se/EV2fUajFpKVMq1-ldBN94fcBsKot6-n9FF3dxAUt6z1Kcw</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
 </sst>
@@ -2472,23 +2520,23 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="149.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="42.42578125" style="62" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" style="62" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="149.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="57.54296875" style="62" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" style="62" customWidth="1"/>
+    <col min="7" max="7" width="28.26953125" style="62" customWidth="1"/>
+    <col min="8" max="8" width="35.7265625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -2511,7 +2559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
@@ -2522,7 +2570,7 @@
       <c r="F2" s="58"/>
       <c r="G2" s="59"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
@@ -2533,10 +2581,10 @@
       <c r="F3" s="60"/>
       <c r="G3" s="61"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -2545,7 +2593,7 @@
       <c r="D5" s="16"/>
       <c r="E5" s="63"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
@@ -2558,7 +2606,7 @@
       <c r="F6" s="58"/>
       <c r="G6" s="59"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>3</v>
       </c>
@@ -2571,7 +2619,7 @@
       <c r="F7" s="64"/>
       <c r="G7" s="65"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
         <v>4</v>
       </c>
@@ -2584,7 +2632,7 @@
       <c r="F8" s="64"/>
       <c r="G8" s="65"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
@@ -2595,15 +2643,15 @@
       <c r="F9" s="60"/>
       <c r="G9" s="61"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="29" t="s">
         <v>34</v>
       </c>
@@ -2616,7 +2664,7 @@
       <c r="F12" s="58"/>
       <c r="G12" s="59"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="30" t="s">
         <v>35</v>
       </c>
@@ -2627,14 +2675,14 @@
       <c r="F13" s="60"/>
       <c r="G13" s="61"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="68"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -2643,12 +2691,12 @@
       <c r="D15" s="19"/>
       <c r="E15" s="68"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A16" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="49"/>
@@ -2656,7 +2704,7 @@
       <c r="F16" s="58"/>
       <c r="G16" s="59"/>
     </row>
-    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
         <v>49</v>
       </c>
@@ -2673,7 +2721,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="31" t="s">
         <v>18</v>
       </c>
@@ -2684,7 +2732,7 @@
       <c r="F18" s="64"/>
       <c r="G18" s="65"/>
     </row>
-    <row r="19" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A19" s="31" t="s">
         <v>19</v>
       </c>
@@ -2699,7 +2747,7 @@
       </c>
       <c r="G19" s="65"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="31" t="s">
         <v>20</v>
       </c>
@@ -2710,7 +2758,7 @@
       <c r="F20" s="64"/>
       <c r="G20" s="65"/>
     </row>
-    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="31" t="s">
         <v>21</v>
       </c>
@@ -2725,7 +2773,7 @@
       </c>
       <c r="G21" s="65"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="31" t="s">
         <v>24</v>
       </c>
@@ -2738,7 +2786,7 @@
       <c r="F22" s="64"/>
       <c r="G22" s="65"/>
     </row>
-    <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="32" t="s">
         <v>25</v>
       </c>
@@ -2751,7 +2799,7 @@
       <c r="F23" s="64"/>
       <c r="G23" s="65"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="33" t="s">
         <v>31</v>
       </c>
@@ -2764,7 +2812,7 @@
       <c r="F24" s="60"/>
       <c r="G24" s="61"/>
     </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -2774,7 +2822,7 @@
       <c r="G25" s="68"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -2783,7 +2831,7 @@
       <c r="D26" s="19"/>
       <c r="E26" s="68"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>23</v>
       </c>
@@ -2797,7 +2845,7 @@
       <c r="G27" s="58"/>
       <c r="H27" s="12"/>
     </row>
-    <row r="28" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="34" t="s">
         <v>37</v>
       </c>
@@ -2813,7 +2861,7 @@
       <c r="G28" s="64"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="35" t="s">
         <v>38</v>
       </c>
@@ -2821,13 +2869,13 @@
       <c r="C29" s="22"/>
       <c r="D29" s="52"/>
       <c r="E29" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" s="64"/>
       <c r="G29" s="64"/>
       <c r="H29" s="18"/>
     </row>
-    <row r="30" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="54" t="s">
         <v>39</v>
       </c>
@@ -2838,7 +2886,7 @@
         <v>63</v>
       </c>
       <c r="F30" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="60" t="s">
         <v>66</v>
@@ -2847,12 +2895,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="23"/>
       <c r="E31" s="63"/>
       <c r="F31" s="63"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
@@ -2861,7 +2909,7 @@
       <c r="E32" s="72"/>
       <c r="F32" s="63"/>
     </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="29" t="s">
         <v>15</v>
       </c>
@@ -2875,7 +2923,7 @@
       <c r="G33" s="58"/>
       <c r="H33" s="12"/>
     </row>
-    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="31" t="s">
         <v>32</v>
       </c>
@@ -2889,7 +2937,7 @@
       <c r="G34" s="64"/>
       <c r="H34" s="18"/>
     </row>
-    <row r="35" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A35" s="31" t="s">
         <v>17</v>
       </c>
@@ -2907,7 +2955,7 @@
       </c>
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="31" t="s">
         <v>22</v>
       </c>
@@ -2921,13 +2969,13 @@
       <c r="G36" s="64"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A37" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="41"/>
       <c r="C37" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D37" s="48"/>
       <c r="E37" s="74" t="s">
@@ -2941,7 +2989,7 @@
       </c>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="55"/>
       <c r="B38" s="42"/>
       <c r="C38" s="38" t="s">
@@ -2953,7 +3001,7 @@
       <c r="G38" s="64"/>
       <c r="H38" s="18"/>
     </row>
-    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="56"/>
       <c r="B39" s="43"/>
       <c r="C39" s="39" t="s">
@@ -2965,7 +3013,7 @@
       <c r="G39" s="64"/>
       <c r="H39" s="18"/>
     </row>
-    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="37" t="s">
         <v>28</v>
       </c>
@@ -2979,7 +3027,7 @@
       <c r="G40" s="64"/>
       <c r="H40" s="18"/>
     </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="34" t="s">
         <v>29</v>
       </c>
@@ -2993,7 +3041,7 @@
       <c r="G41" s="64"/>
       <c r="H41" s="18"/>
     </row>
-    <row r="42" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A42" s="34" t="s">
         <v>33</v>
       </c>
@@ -3013,7 +3061,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="32" t="s">
         <v>27</v>
       </c>
@@ -3027,7 +3075,7 @@
       <c r="G43" s="64"/>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="33" t="s">
         <v>26</v>
       </c>
@@ -3041,16 +3089,16 @@
       <c r="G44" s="60"/>
       <c r="H44" s="14"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E45" s="63"/>
       <c r="F45" s="63"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E46" s="63"/>
       <c r="F46" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>